<commit_message>
qc sires and dames of the pedigree, create csv's for the 12 missing pedigree from hao chen, notes for pedigree questions for wfu
</commit_message>
<xml_diff>
--- a/CREATE/rows_with_F_sire.xlsx
+++ b/CREATE/rows_with_F_sire.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t xml:space="preserve">excel_row</t>
   </si>
@@ -59,151 +59,181 @@
     <t xml:space="preserve">dam_sw_id</t>
   </si>
   <si>
-    <t xml:space="preserve">3278</t>
+    <t xml:space="preserve">3342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73154_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRN HOOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
   </si>
   <si>
     <t xml:space="preserve">72772_4</t>
   </si>
   <si>
-    <t xml:space="preserve">BROWN HOOD</t>
+    <t xml:space="preserve">WHSM0503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSM0405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSF0403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3343</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73192_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALBINO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSM0504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSM0417</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSF0404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73512_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72905_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72801_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSM0517B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBRB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73505_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73309_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73347_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSM0561B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73556_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSM0503B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73154_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BROWN</t>
   </si>
   <si>
     <t xml:space="preserve">F</t>
   </si>
   <si>
-    <t xml:space="preserve">72623_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72527_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSF0403</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSM0334</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSF0303</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3282</t>
+    <t xml:space="preserve">3409</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73192_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSF0504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73504_4</t>
   </si>
   <si>
     <t xml:space="preserve">72945_1</t>
   </si>
   <si>
-    <t xml:space="preserve">BROWN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72543_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72531_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSF0407</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSM0320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSF0307</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3290</t>
+    <t xml:space="preserve">72797_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSF0507B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73511_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLACK HOOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73337_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73332_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSF0551B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73546_1</t>
   </si>
   <si>
     <t xml:space="preserve">72794_2</t>
   </si>
   <si>
-    <t xml:space="preserve">72625_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72539_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSF0416</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSM0335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSF0316</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3292</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72905_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72536_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72540_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSF0417</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSM0313</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSF0317</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3325</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73337_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALBINO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73335_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73336_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHSF0451</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73309_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BLACK HOOD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73307_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73308_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WSHF0461</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2700</t>
+    <t xml:space="preserve">72790_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHSF0516B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTRB</t>
   </si>
 </sst>
 </file>
@@ -602,34 +632,34 @@
         <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2"/>
       <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>24</v>
-      </c>
-      <c r="O2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -638,37 +668,37 @@
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="J3"/>
       <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" t="s">
         <v>31</v>
-      </c>
-      <c r="L3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -677,37 +707,33 @@
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J4"/>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" t="s">
-        <v>42</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="N4"/>
+      <c r="O4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -716,37 +742,33 @@
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J5"/>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" t="s">
-        <v>48</v>
-      </c>
-      <c r="O5" t="s">
-        <v>49</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="N5"/>
+      <c r="O5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
@@ -755,58 +777,206 @@
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="J6"/>
       <c r="K6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="M6" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="N6"/>
       <c r="O6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J7"/>
       <c r="K7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8"/>
+      <c r="K8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9"/>
+      <c r="K9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9"/>
+      <c r="O9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
         <v>62</v>
       </c>
-      <c r="L7" t="s">
+      <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="M7" t="s">
-        <v>40</v>
-      </c>
-      <c r="N7"/>
-      <c r="O7"/>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10"/>
+      <c r="O10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11"/>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" t="s">
+        <v>73</v>
+      </c>
+      <c r="N11"/>
+      <c r="O11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>